<commit_message>
New rounding for VAT tables
</commit_message>
<xml_diff>
--- a/final-outputs/Table C Consumption.xlsx
+++ b/final-outputs/Table C Consumption.xlsx
@@ -344,100 +344,100 @@
     <t>VAT/Sales Tax Threshold (a)</t>
   </si>
   <si>
-    <t>$50,950.98</t>
-  </si>
-  <si>
-    <t>$37,457.44</t>
-  </si>
-  <si>
-    <t>$31,109.15</t>
-  </si>
-  <si>
-    <t>$23,975.89</t>
-  </si>
-  <si>
-    <t>$0.00</t>
-  </si>
-  <si>
-    <t>$76,296.54</t>
-  </si>
-  <si>
-    <t>$6,907.64</t>
-  </si>
-  <si>
-    <t>$72,611.89</t>
-  </si>
-  <si>
-    <t>$11,062.41</t>
-  </si>
-  <si>
-    <t>$103,912.92</t>
-  </si>
-  <si>
-    <t>$22,456.28</t>
-  </si>
-  <si>
-    <t>$16,710.70</t>
-  </si>
-  <si>
-    <t>$57,601.50</t>
-  </si>
-  <si>
-    <t>$14,202.16</t>
-  </si>
-  <si>
-    <t>$92,218.14</t>
-  </si>
-  <si>
-    <t>$26,132.39</t>
-  </si>
-  <si>
-    <t>$90,380.96</t>
-  </si>
-  <si>
-    <t>$100,407.57</t>
-  </si>
-  <si>
-    <t>$34,205.49</t>
-  </si>
-  <si>
-    <t>$79,773.92</t>
-  </si>
-  <si>
-    <t>$97,563.09</t>
-  </si>
-  <si>
-    <t>$33,690.38</t>
-  </si>
-  <si>
-    <t>$1,650.19</t>
-  </si>
-  <si>
-    <t>$40,813.16</t>
-  </si>
-  <si>
-    <t>$4,916.69</t>
-  </si>
-  <si>
-    <t>$111,214.73</t>
-  </si>
-  <si>
-    <t>$16,886.44</t>
-  </si>
-  <si>
-    <t>$100,763.36</t>
-  </si>
-  <si>
-    <t>$83,256.74</t>
-  </si>
-  <si>
-    <t>$3,296.89</t>
-  </si>
-  <si>
-    <t>$81,953.38</t>
-  </si>
-  <si>
-    <t>$119,167.29</t>
+    <t>$50,951</t>
+  </si>
+  <si>
+    <t>$37,457</t>
+  </si>
+  <si>
+    <t>$31,109</t>
+  </si>
+  <si>
+    <t>$23,976</t>
+  </si>
+  <si>
+    <t>$0</t>
+  </si>
+  <si>
+    <t>$76,297</t>
+  </si>
+  <si>
+    <t>$6,908</t>
+  </si>
+  <si>
+    <t>$72,612</t>
+  </si>
+  <si>
+    <t>$11,062</t>
+  </si>
+  <si>
+    <t>$103,913</t>
+  </si>
+  <si>
+    <t>$22,456</t>
+  </si>
+  <si>
+    <t>$16,711</t>
+  </si>
+  <si>
+    <t>$57,602</t>
+  </si>
+  <si>
+    <t>$14,202</t>
+  </si>
+  <si>
+    <t>$92,218</t>
+  </si>
+  <si>
+    <t>$26,132</t>
+  </si>
+  <si>
+    <t>$90,381</t>
+  </si>
+  <si>
+    <t>$100,408</t>
+  </si>
+  <si>
+    <t>$34,205</t>
+  </si>
+  <si>
+    <t>$79,774</t>
+  </si>
+  <si>
+    <t>$97,563</t>
+  </si>
+  <si>
+    <t>$33,690</t>
+  </si>
+  <si>
+    <t>$1,650</t>
+  </si>
+  <si>
+    <t>$40,813</t>
+  </si>
+  <si>
+    <t>$4,917</t>
+  </si>
+  <si>
+    <t>$111,215</t>
+  </si>
+  <si>
+    <t>$16,886</t>
+  </si>
+  <si>
+    <t>$100,763</t>
+  </si>
+  <si>
+    <t>$83,257</t>
+  </si>
+  <si>
+    <t>$3,297</t>
+  </si>
+  <si>
+    <t>$81,953</t>
+  </si>
+  <si>
+    <t>$119,167</t>
   </si>
   <si>
     <t>VAT/Sales Tax Base as a Percent of Total Consumption</t>

</xml_diff>